<commit_message>
Add items file download when is not template
</commit_message>
<xml_diff>
--- a/test/resources/items.xlsx
+++ b/test/resources/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbrunetta/Documents/Projects/ifoody-api/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64662CF-E765-F443-B1F0-C4514B3B090C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92238B0E-C78B-FA4E-8616-DB52C426D0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+  <si>
+    <t>Code</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -53,13 +56,22 @@
   </si>
   <si>
     <t>Pão cervejinha , hambúrguer de gado 180g, queijo muçarela, alface, bacon, tomate e molho chimichurri. Um acompanhamento à escolha: anel de cebola ou batata palito.</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>0003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +85,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,11 +128,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,22 +449,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="138.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="138.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -436,50 +474,62 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
+      <c r="E4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>